<commit_message>
Take works now, but some glitches
</commit_message>
<xml_diff>
--- a/ErwinLootTable.xlsx
+++ b/ErwinLootTable.xlsx
@@ -2,43 +2,27 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://twoia-my.sharepoint.com/personal/matt_revov_co_za/Documents/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://twoia-my.sharepoint.com/personal/matt_revov_co_za/Documents/Documents/Personal/ErwinApp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="186" documentId="8_{8CEA14CE-7891-404C-AB67-961C290F49DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B02E4400-1F63-4097-972C-016AFF759FCE}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_C9692D42A2674189A92644E4E71E4A9265F07DFD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0735FFC-96DF-4EE5-9E70-EE2C6BF85303}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{9CA590E0-14FF-4FBD-B7FF-65CDD095F929}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Loot" sheetId="1" r:id="rId1"/>
     <sheet name="Players" sheetId="2" r:id="rId2"/>
     <sheet name="Loot box sizes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="64">
   <si>
     <t>Item</t>
   </si>
@@ -46,6 +30,18 @@
     <t>Description</t>
   </si>
   <si>
+    <t>Value(GP)</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Item scarecity</t>
+  </si>
+  <si>
     <t>Gold Coin</t>
   </si>
   <si>
@@ -70,9 +66,6 @@
     <t>Mined from Shuriman deserts, glows softly with solar energy.</t>
   </si>
   <si>
-    <t>Value(GP)</t>
-  </si>
-  <si>
     <t>Hex Crystal Shard</t>
   </si>
   <si>
@@ -169,18 +162,33 @@
     <t>Player 2</t>
   </si>
   <si>
+    <t>MrTinMan</t>
+  </si>
+  <si>
     <t>Loot</t>
   </si>
   <si>
-    <t>Max</t>
-  </si>
-  <si>
     <t>Qty</t>
   </si>
   <si>
     <t>Loot box name</t>
   </si>
   <si>
+    <t>Max total items</t>
+  </si>
+  <si>
+    <t>Min box value</t>
+  </si>
+  <si>
+    <t>Max box value</t>
+  </si>
+  <si>
+    <t>Min scarecity</t>
+  </si>
+  <si>
+    <t>Max scarecity</t>
+  </si>
+  <si>
     <t>purse</t>
   </si>
   <si>
@@ -202,34 +210,10 @@
     <t>grande chest</t>
   </si>
   <si>
+    <t>legendary chest</t>
+  </si>
+  <si>
     <t>wrecked ship</t>
-  </si>
-  <si>
-    <t>Max total items</t>
-  </si>
-  <si>
-    <t>Item scarecity</t>
-  </si>
-  <si>
-    <t>Max box value</t>
-  </si>
-  <si>
-    <t>Min box value</t>
-  </si>
-  <si>
-    <t>Min scarecity</t>
-  </si>
-  <si>
-    <t>Max scarecity</t>
-  </si>
-  <si>
-    <t>legendary chest</t>
-  </si>
-  <si>
-    <t>Weight</t>
-  </si>
-  <si>
-    <t>MrTinMan</t>
   </si>
 </sst>
 </file>
@@ -245,10 +229,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <b/>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -259,7 +242,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -267,14 +250,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -609,7 +610,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34403936-9877-4FFE-9283-46239C23BCFB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -632,24 +633,24 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -666,10 +667,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>0.1</v>
@@ -686,10 +687,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>0.01</v>
@@ -706,10 +707,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>75</v>
@@ -726,10 +727,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <v>150</v>
@@ -746,10 +747,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>250</v>
@@ -766,10 +767,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C8">
         <v>120</v>
@@ -786,10 +787,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C9">
         <v>500</v>
@@ -806,10 +807,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C10">
         <v>180</v>
@@ -826,10 +827,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C11">
         <v>800</v>
@@ -846,10 +847,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C12">
         <v>1000</v>
@@ -866,10 +867,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C13">
         <v>200</v>
@@ -886,10 +887,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C14">
         <v>400</v>
@@ -906,10 +907,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C15">
         <v>350</v>
@@ -926,10 +927,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C16">
         <v>850</v>
@@ -946,10 +947,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C17">
         <v>300</v>
@@ -966,10 +967,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C18">
         <v>600</v>
@@ -986,10 +987,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C19">
         <v>1200</v>
@@ -1006,10 +1007,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C20">
         <v>90</v>
@@ -1030,116 +1031,183 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5AA81F0-FE2B-407E-BF6D-CB2A96CAB7ED}">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:B1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>0</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4">
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
       <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>1000</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7">
         <v>4</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
+    <mergeCell ref="G1:H1"/>
     <mergeCell ref="E1:F1"/>
   </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45600D8A-42F4-491A-BF70-7539648493F6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1157,27 +1225,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -1197,7 +1265,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1217,7 +1285,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B4">
         <v>6</v>
@@ -1237,7 +1305,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1257,7 +1325,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B6">
         <v>6</v>
@@ -1277,7 +1345,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B7">
         <v>8</v>
@@ -1297,7 +1365,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B8">
         <v>10</v>
@@ -1317,7 +1385,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1337,7 +1405,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B10">
         <v>20</v>

</xml_diff>